<commit_message>
Modify database table documentation
</commit_message>
<xml_diff>
--- a/dbm/Relation.xlsx
+++ b/dbm/Relation.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7273B6B5-8419-4E25-B5ED-0E2A365A39BD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802CCB93-9518-4383-9ED9-23486AE544E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="user" sheetId="1" r:id="rId1"/>
@@ -116,25 +116,24 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>user_id(FK)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>owner_id(FK)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -143,7 +142,7 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -151,14 +150,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -220,7 +219,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -504,17 +503,17 @@
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="5" width="16.625" customWidth="1"/>
+    <col min="2" max="5" width="16.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5">
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5">
       <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
@@ -528,7 +527,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -546,20 +545,20 @@
   <dimension ref="B3:C5"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="3" width="16.625" customWidth="1"/>
+    <col min="2" max="3" width="16.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3">
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3">
       <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
@@ -567,7 +566,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
     </row>
@@ -585,17 +584,17 @@
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="6" width="16.625" customWidth="1"/>
+    <col min="2" max="6" width="16.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6">
       <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6">
       <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
@@ -612,14 +611,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6">
       <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
@@ -627,7 +626,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6">
       <c r="C8" s="1" t="s">
         <v>15</v>
       </c>
@@ -635,7 +634,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6">
       <c r="C9" s="1" t="s">
         <v>17</v>
       </c>
@@ -643,7 +642,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6">
       <c r="C10" s="1" t="s">
         <v>19</v>
       </c>
@@ -651,7 +650,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6">
       <c r="C11" s="1" t="s">
         <v>21</v>
       </c>

</xml_diff>